<commit_message>
Se termino el laboratorio del reloj
</commit_message>
<xml_diff>
--- a/FP1-M2/Laboratorio,reloj.xlsx
+++ b/FP1-M2/Laboratorio,reloj.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>hour</t>
   </si>
@@ -34,14 +34,14 @@
   <si>
     <t>dura</t>
   </si>
-  <si>
-    <t>=</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,10 +71,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,15 +356,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3:K6"/>
+  <dimension ref="F3:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>0</v>
       </c>
@@ -373,11 +377,23 @@
       <c r="H3">
         <v>23</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <f>G3+J6</f>
+        <v>13.266666666666666</v>
+      </c>
+      <c r="K3" s="1">
+        <f>H3+K6</f>
+        <v>34.666666666666664</v>
+      </c>
+      <c r="L3" s="1">
+        <f>I3+L6</f>
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>1</v>
       </c>
@@ -387,8 +403,23 @@
       <c r="H4">
         <v>58</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f>(G4+G5)</f>
+        <v>76</v>
+      </c>
+      <c r="K4">
+        <f>(H4+H5)</f>
+        <v>700</v>
+      </c>
+      <c r="L4">
+        <f>(I4+I5)</f>
+        <v>2940</v>
+      </c>
     </row>
-    <row r="5" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -398,15 +429,32 @@
       <c r="H5">
         <v>642</v>
       </c>
+      <c r="I5">
+        <v>2939</v>
+      </c>
     </row>
-    <row r="6" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:12" x14ac:dyDescent="0.25">
       <c r="G6" s="2">
         <v>0.55277777777777781</v>
       </c>
       <c r="H6" s="2">
         <v>0.44444444444444442</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="I6" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <f>J4/60</f>
+        <v>1.2666666666666666</v>
+      </c>
+      <c r="K6" s="3">
+        <f>K4/60</f>
+        <v>11.666666666666666</v>
+      </c>
+      <c r="L6" s="3">
+        <f>L4/60</f>
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>